<commit_message>
Added more icons and UI elements. Working on charting. Added CSV export of data buffer.
</commit_message>
<xml_diff>
--- a/DJet ECU Tester/PCB/DJetECUTester/BOM.xlsx
+++ b/DJet ECU Tester/PCB/DJetECUTester/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34800" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="DJetECUTester" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
   <si>
     <t>Item</t>
   </si>
@@ -57,397 +57,316 @@
     <t>Capacitor_SMD:CP_Elec_4x5.8</t>
   </si>
   <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>Device:C</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>680uF e</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:CP_Elec_10x10.5</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>220uF e</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:CP_Elec_8x6.5</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>4.7uF 16V e</t>
+  </si>
+  <si>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>Device:D</t>
+  </si>
+  <si>
+    <t>Britishideas:SOD-123</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>B360A-13-F</t>
+  </si>
+  <si>
+    <t>Device:D_Schottky</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_SMA</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>Device:LED</t>
+  </si>
+  <si>
+    <t>LED_SMD:LED_PLCC-2</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>MI0805K400R-10</t>
+  </si>
+  <si>
+    <t>Device:Ferrite_Bead</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>USB_B_Mini</t>
+  </si>
+  <si>
+    <t>DJetECUTester-rescue:USB_B_Mini-Connector</t>
+  </si>
+  <si>
+    <t>Connector_USB:USB_Mini-B_Wuerth_65100516121_Horizontal</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>33uH</t>
+  </si>
+  <si>
+    <t>Device:L</t>
+  </si>
+  <si>
+    <t>Britishideas:Wurth-WE-LQS-Inductor</t>
+  </si>
+  <si>
+    <t>680uH</t>
+  </si>
+  <si>
+    <t>Britishideas:Inductor-MSS1210-684KED</t>
+  </si>
+  <si>
+    <t>MSS1210-684KED</t>
+  </si>
+  <si>
+    <t>MMBT2222ALT1G</t>
+  </si>
+  <si>
+    <t>Transistor_BJT:MMBT3904</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>MMBT3906LT1G</t>
+  </si>
+  <si>
+    <t>Device:Q_PNP_BEC</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>Device:R</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>11k</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>4k2</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>2k6</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>CRCW1206680RFKEAHP</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ATmega328P</t>
+  </si>
+  <si>
+    <t>BritishIdeas:ATmega328P</t>
+  </si>
+  <si>
+    <t>Package_QFP:LQFP-32_7x7mm_P0.8mm</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AUR</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>LM2596S-5</t>
+  </si>
+  <si>
+    <t>Regulator_Switching:LM2596S-5</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:TO-263-5_TabPin3</t>
+  </si>
+  <si>
+    <t>LM2596S-5.0/NOPB</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>Interface_USB:FT232RL</t>
+  </si>
+  <si>
+    <t>Package_SO:SSOP-28_5.3x10.2mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>FT232RL-REEL</t>
+  </si>
+  <si>
+    <t>MCP41HV51-502E-ST</t>
+  </si>
+  <si>
+    <t>BritishIdeas:MCP41HV51-502E-ST</t>
+  </si>
+  <si>
+    <t>Package_SO:TSSOP-14_4.4x5mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>MCP41HV51-502E/ST</t>
+  </si>
+  <si>
+    <t>MCP41HV31-502E/ST</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>MCP23S08T-E_SO</t>
+  </si>
+  <si>
+    <t>BritishIdeas:MCP23S08T-E_SO</t>
+  </si>
+  <si>
+    <t>Package_SO:SOIC-18W_7.5x11.6mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>FA-238 16.0000MB-C3</t>
+  </si>
+  <si>
+    <t>Device:Crystal_GND24</t>
+  </si>
+  <si>
+    <t>Britishideas:FA-238</t>
+  </si>
+  <si>
     <t>C2, C9, C11, C13, C14, C15, C16, C17, C18, C19, C20</t>
   </si>
   <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>Device:C</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_0805_2012Metric</t>
-  </si>
-  <si>
     <t>C3, C6</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
     <t>C4, C5</t>
   </si>
   <si>
-    <t>18pF</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>680uF e</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:CP_Elec_10x10.5</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>220uF e</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:CP_Elec_8x6.5</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>4.7uF 16V e</t>
-  </si>
-  <si>
-    <t>D1, D4, D5, D6, D7, D9, D10</t>
-  </si>
-  <si>
-    <t>MBR0520LT1G</t>
-  </si>
-  <si>
-    <t>Device:D</t>
-  </si>
-  <si>
-    <t>Britishideas:SOD-123</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>B360A-13-F</t>
-  </si>
-  <si>
-    <t>Device:D_Schottky</t>
-  </si>
-  <si>
-    <t>Diode_SMD:D_SMA</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>PWR</t>
-  </si>
-  <si>
-    <t>Device:LED</t>
-  </si>
-  <si>
-    <t>LED_SMD:LED_PLCC-2</t>
+    <t>D1, D4, D5, D6, D7, D10</t>
   </si>
   <si>
     <t>D8, D11</t>
   </si>
   <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>FB1</t>
-  </si>
-  <si>
-    <t>MI0805K400R-10</t>
-  </si>
-  <si>
-    <t>Device:Ferrite_Bead</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>ECU1</t>
-  </si>
-  <si>
-    <t>Connector:Screw_Terminal_01x08</t>
-  </si>
-  <si>
-    <t>Britishideas:PhoenixContact_COMBICON_PT_8</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>USB_B_Mini</t>
-  </si>
-  <si>
-    <t>DJetECUTester-rescue:USB_B_Mini-Connector</t>
-  </si>
-  <si>
-    <t>Connector_USB:USB_Mini-B_Wuerth_65100516121_Horizontal</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>12V 4A IN (5.5/2.5)</t>
-  </si>
-  <si>
-    <t>Connector:Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>Connector_BarrelJack:BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>12V IN</t>
-  </si>
-  <si>
-    <t>Connector:Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>Britishideas:PhoenixContact_COMBICON_MKDSN_2</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>MPS</t>
-  </si>
-  <si>
-    <t>Connector:Screw_Terminal_01x04</t>
-  </si>
-  <si>
-    <t>Britishideas:PhoenixContact_COMBICON_PT_4</t>
-  </si>
-  <si>
-    <t>J7, J8</t>
-  </si>
-  <si>
-    <t>Conn_01x01</t>
-  </si>
-  <si>
-    <t>Connector_Generic:Conn_01x01</t>
-  </si>
-  <si>
-    <t>Britishideas:tabconnector-63849-1</t>
-  </si>
-  <si>
-    <t>63849-1</t>
-  </si>
-  <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>ECU2</t>
-  </si>
-  <si>
-    <t>Connector:Screw_Terminal_01x10</t>
-  </si>
-  <si>
-    <t>Britishideas:PhoenixContact_COMBICON_PT_10</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>ECU3</t>
-  </si>
-  <si>
-    <t>Connector:Screw_Terminal_01x07</t>
-  </si>
-  <si>
-    <t>Britishideas:PhoenixContact_COMBICON_PT_7</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>33uH</t>
-  </si>
-  <si>
-    <t>Device:L</t>
-  </si>
-  <si>
-    <t>Britishideas:Wurth-WE-LQS-Inductor</t>
-  </si>
-  <si>
     <t>L2, L3, L4, L5, L6, L7, L8, L9, L10, L11, L12, L13, L14, L15, L16, L17</t>
   </si>
   <si>
-    <t>680uH</t>
-  </si>
-  <si>
-    <t>Britishideas:Inductor-MSS1210-684KED</t>
-  </si>
-  <si>
-    <t>MSS1210-684KED</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12</t>
-  </si>
-  <si>
-    <t>MMBT2222ALT1G</t>
-  </si>
-  <si>
-    <t>Transistor_BJT:MMBT3904</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD:SOT-23</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R6, R44</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>Device:R</t>
-  </si>
-  <si>
-    <t>R5, R9, R10, R13, R14, R19, R20, R23, R24, R25, R26, R27, R32, R33, R34, R35, R36, R38, R40, R42, R52, R53</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R7, R8, R11, R12, R17, R18, R21, R22</t>
-  </si>
-  <si>
-    <t>1k</t>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R6, R44, R55</t>
+  </si>
+  <si>
+    <t>R5, R9, R10, R13, R14, R19, R20, R23, R24, R25, R26, R27, R32, R33, R34, R35, R36, R38, R40, R42, R52, R53, R58</t>
+  </si>
+  <si>
+    <t>R7, R8, R11, R12, R17, R18, R21, R22, R48, R59</t>
   </si>
   <si>
     <t>R15, R16, R28, R29, R30, R31, R45</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>R37, R39, R41, R43</t>
   </si>
   <si>
-    <t>11k</t>
-  </si>
-  <si>
-    <t>R46, R47, R50, R51</t>
-  </si>
-  <si>
-    <t>Device:R_POT</t>
-  </si>
-  <si>
-    <t>Britishideas:Potentometer_Bourns_PV36W</t>
-  </si>
-  <si>
-    <t>PV36W500C01B00</t>
-  </si>
-  <si>
-    <t>R48, R49</t>
-  </si>
-  <si>
-    <t>4k2</t>
-  </si>
-  <si>
-    <t>R54</t>
-  </si>
-  <si>
-    <t>2k6</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>ATmega328P</t>
-  </si>
-  <si>
-    <t>BritishIdeas:ATmega328P</t>
-  </si>
-  <si>
-    <t>Package_QFP:LQFP-32_7x7mm_P0.8mm</t>
-  </si>
-  <si>
-    <t>ATMEGA328P-AUR</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>LM2596S-5</t>
-  </si>
-  <si>
-    <t>Regulator_Switching:LM2596S-5</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD:TO-263-5_TabPin3</t>
-  </si>
-  <si>
-    <t>LM2596S-5.0/NOPB</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>FT232RL</t>
-  </si>
-  <si>
-    <t>Interface_USB:FT232RL</t>
-  </si>
-  <si>
-    <t>Package_SO:SSOP-28_5.3x10.2mm_P0.65mm</t>
-  </si>
-  <si>
-    <t>FT232RL-REEL</t>
+    <t>R57, R60</t>
   </si>
   <si>
     <t>U4, U5, U7</t>
-  </si>
-  <si>
-    <t>MCP41HV51-502E-ST</t>
-  </si>
-  <si>
-    <t>BritishIdeas:MCP41HV51-502E-ST</t>
-  </si>
-  <si>
-    <t>Package_SO:TSSOP-14_4.4x5mm_P0.65mm</t>
-  </si>
-  <si>
-    <t>MCP41HV51-502E/ST</t>
-  </si>
-  <si>
-    <t>MCP41HV31-502E/ST</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>MCP23S08T-E_SO</t>
-  </si>
-  <si>
-    <t>BritishIdeas:MCP23S08T-E_SO</t>
-  </si>
-  <si>
-    <t>Package_SO:SOIC-18W_7.5x11.6mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>FA-238 16.0000MB-C3</t>
-  </si>
-  <si>
-    <t>Device:Crystal_GND24</t>
-  </si>
-  <si>
-    <t>Britishideas:FA-238</t>
-  </si>
-  <si>
-    <t>5194TR</t>
-  </si>
-  <si>
-    <t>5195TR</t>
   </si>
 </sst>
 </file>
@@ -931,9 +850,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1255,21 +1173,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1327,16 +1245,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1347,16 +1265,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1367,16 +1285,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1387,16 +1305,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1407,16 +1325,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1427,16 +1345,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1447,10 +1365,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1464,22 +1382,22 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1490,19 +1408,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1513,16 +1431,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1533,16 +1451,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,595 +1471,455 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G15">
-        <v>1935831</v>
+        <v>65100516121</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>74404063330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>27</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
+      <c r="G17" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E18" t="s">
         <v>55</v>
       </c>
-      <c r="G16">
-        <v>65100516121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F18" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D19" t="s">
         <v>58</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="1">
-        <v>694108000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E20" t="s">
         <v>61</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="G18">
-        <v>1729018</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="F19" t="s">
+      <c r="D25" t="s">
         <v>67</v>
       </c>
-      <c r="G19">
-        <v>1935792</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20">
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28">
+        <v>680</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="G28" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>74</v>
       </c>
-      <c r="E21" t="s">
+      <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E29" t="s">
         <v>76</v>
       </c>
-      <c r="G21">
-        <v>1935242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="F29" t="s">
         <v>77</v>
       </c>
-      <c r="D22" t="s">
+      <c r="G29" t="s">
         <v>78</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>79</v>
       </c>
-      <c r="F22" t="s">
+      <c r="D30" t="s">
         <v>80</v>
       </c>
-      <c r="G22">
-        <v>1935213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E30" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F30" t="s">
         <v>82</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G30" t="s">
         <v>83</v>
       </c>
-      <c r="F23" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>84</v>
       </c>
-      <c r="G23">
-        <v>74404063330</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E31" t="s">
         <v>86</v>
       </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="F31" t="s">
         <v>87</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
         <v>89</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E32" t="s">
         <v>90</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F32" t="s">
         <v>91</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G32" t="s">
         <v>92</v>
       </c>
-      <c r="G25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="H32" t="s">
         <v>93</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D33" t="s">
         <v>95</v>
       </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>22</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F33" t="s">
         <v>97</v>
       </c>
-      <c r="E27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D34" t="s">
         <v>99</v>
       </c>
-      <c r="E28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E34" t="s">
         <v>100</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F34" t="s">
         <v>101</v>
       </c>
-      <c r="E29" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>33</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31">
-        <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>35</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>36</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" t="s">
-        <v>115</v>
-      </c>
       <c r="G34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" t="s">
-        <v>120</v>
-      </c>
-      <c r="G35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" t="s">
-        <v>123</v>
-      </c>
-      <c r="E36" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" t="s">
-        <v>128</v>
-      </c>
-      <c r="E37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H37" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>40</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>133</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
-      </c>
-      <c r="E38" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>41</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>